<commit_message>
solar and wind for WestEu
</commit_message>
<xml_diff>
--- a/version_oct_2023/New_DietData.xlsx
+++ b/version_oct_2023/New_DietData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aaudk-my.sharepoint.com/personal/vn73vs_plan_aau_dk/Documents/Research RU/Felix-Model/version_oct_2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub-my.sharepoint.com/personal/yequanliang_iiasa_ac_at/Documents/research_iiasa/Felix-Model/version_oct_2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_5523B6F1FF37483A581E8314AEA41110AD641C97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC36E04A-E75F-4D2B-9F61-C06E4A766D2E}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_5523B6F1FF37483A581E8314AEA41110AD641C97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8349FEE-5497-45A2-873E-05C1F552EDCD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackgroundData" sheetId="1" r:id="rId1"/>
@@ -5180,29 +5180,29 @@
       <selection pane="topRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="6" width="14.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="9" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="3" max="6" width="14.875" customWidth="1"/>
+    <col min="7" max="7" width="16.875" customWidth="1"/>
+    <col min="8" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" customWidth="1"/>
-    <col min="15" max="15" width="22.88671875" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" customWidth="1"/>
-    <col min="17" max="18" width="17.88671875" customWidth="1"/>
-    <col min="19" max="19" width="18.44140625" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.625" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="13" max="13" width="17.625" customWidth="1"/>
+    <col min="14" max="14" width="14.875" customWidth="1"/>
+    <col min="15" max="15" width="22.875" customWidth="1"/>
+    <col min="16" max="16" width="19.625" customWidth="1"/>
+    <col min="17" max="18" width="17.875" customWidth="1"/>
+    <col min="19" max="19" width="18.5" customWidth="1"/>
+    <col min="20" max="20" width="15.375" customWidth="1"/>
     <col min="21" max="21" width="15" customWidth="1"/>
-    <col min="22" max="22" width="14.5546875" customWidth="1"/>
-    <col min="26" max="26" width="13.109375" customWidth="1"/>
+    <col min="22" max="22" width="14.5" customWidth="1"/>
+    <col min="26" max="26" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="16.3" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="133" t="s">
         <v>33</v>
@@ -5229,7 +5229,7 @@
       <c r="R1" s="97"/>
       <c r="S1" s="50"/>
     </row>
-    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="72" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
         <v>5</v>
       </c>
@@ -5343,7 +5343,7 @@
       <c r="S3" s="77"/>
       <c r="W3" s="109"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
@@ -5434,7 +5434,7 @@
         <v>32.583399407756325</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>32.49</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>33.020000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="65" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>48</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>1.3164263009192065</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>1.41</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -5960,7 +5960,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
@@ -6188,7 +6188,7 @@
         <v>0.46849690478573225</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>20</v>
       </c>
@@ -6408,7 +6408,7 @@
       <c r="Y17" s="49"/>
       <c r="Z17" s="49"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>7.2355585182809462E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>22</v>
       </c>
@@ -6633,7 +6633,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>23</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>24</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>80</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>0.29572304994050513</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>25</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>9</v>
       </c>
@@ -6999,7 +6999,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>26</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -7119,7 +7119,7 @@
       <c r="U27" s="107"/>
       <c r="W27" s="48"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>10</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>38</v>
       </c>
@@ -7231,7 +7231,7 @@
       <c r="R29" s="57"/>
       <c r="S29" s="77"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>39</v>
       </c>
@@ -7279,7 +7279,7 @@
       <c r="R30" s="57"/>
       <c r="S30" s="77"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>11</v>
       </c>
@@ -7321,7 +7321,7 @@
       <c r="R31" s="22"/>
       <c r="S31" s="77"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J34" t="s">
         <v>120</v>
       </c>
@@ -7330,12 +7330,12 @@
         <v>0.20531348221024776</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -7360,16 +7360,16 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="113" t="s">
         <v>14</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>5.264793108318034E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="113" t="s">
         <v>29</v>
       </c>
@@ -7420,7 +7420,7 @@
         <v>5.264793108318034E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="113" t="s">
         <v>15</v>
       </c>
@@ -7437,7 +7437,7 @@
         <v>1.856203080256946</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="113" t="s">
         <v>16</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>9.4387980556783084</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="113" t="s">
         <v>8</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="114" t="s">
         <v>6</v>
       </c>
@@ -7488,7 +7488,7 @@
         <v>0.71376670261505382</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="115" t="s">
         <v>7</v>
       </c>
@@ -7515,37 +7515,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS96"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="15" topLeftCell="K16" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="19.44140625" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" customWidth="1"/>
-    <col min="15" max="15" width="15.44140625" customWidth="1"/>
-    <col min="16" max="16" width="9.109375" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" customWidth="1"/>
-    <col min="18" max="21" width="9.109375" customWidth="1"/>
-    <col min="22" max="22" width="18.44140625" customWidth="1"/>
-    <col min="24" max="24" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.109375" customWidth="1"/>
-    <col min="27" max="27" width="13.6640625" customWidth="1"/>
-    <col min="29" max="44" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.625" customWidth="1"/>
+    <col min="9" max="9" width="14.125" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="16.5" customWidth="1"/>
+    <col min="12" max="12" width="15.375" customWidth="1"/>
+    <col min="13" max="13" width="12.125" customWidth="1"/>
+    <col min="14" max="14" width="9.125" customWidth="1"/>
+    <col min="15" max="15" width="15.5" customWidth="1"/>
+    <col min="16" max="16" width="9.125" customWidth="1"/>
+    <col min="17" max="17" width="13.125" customWidth="1"/>
+    <col min="18" max="21" width="9.125" customWidth="1"/>
+    <col min="22" max="22" width="18.5" customWidth="1"/>
+    <col min="24" max="24" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.125" customWidth="1"/>
+    <col min="27" max="27" width="13.625" customWidth="1"/>
+    <col min="29" max="44" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="14.95" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B2" s="137" t="s">
         <v>86</v>
       </c>
@@ -7563,7 +7566,7 @@
       </c>
       <c r="I2" s="89"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3" s="85" t="s">
         <v>79</v>
       </c>
@@ -7632,7 +7635,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -7697,7 +7700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -7762,7 +7765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -7827,7 +7830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -7892,7 +7895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -7973,7 +7976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -8054,7 +8057,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -8135,7 +8138,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:28" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -8216,7 +8219,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>74</v>
       </c>
@@ -8233,18 +8236,18 @@
         <v>1.52604801675541</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H13">
         <f>250*0.6/D12</f>
         <v>6.8306010928961755E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="89" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B15" s="50" t="s">
         <v>51</v>
       </c>
@@ -8309,7 +8312,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
         <v>72</v>
       </c>
@@ -8377,7 +8380,7 @@
         <v>2336.9594594594591</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>73</v>
       </c>
@@ -8445,7 +8448,7 @@
         <v>1912.0577395577393</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A19" s="89" t="s">
         <v>75</v>
       </c>
@@ -8453,7 +8456,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A20" s="89" t="s">
         <v>90</v>
       </c>
@@ -8461,7 +8464,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A21" s="90" t="s">
         <v>82</v>
       </c>
@@ -8595,7 +8598,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A22" s="91" t="s">
         <v>77</v>
       </c>
@@ -8771,7 +8774,7 @@
         <v>4.788851351351351E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A23" s="91" t="s">
         <v>78</v>
       </c>
@@ -8947,7 +8950,7 @@
         <v>3.9181511056511058E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A24" s="90" t="s">
         <v>83</v>
       </c>
@@ -8955,7 +8958,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A25" s="91" t="s">
         <v>77</v>
       </c>
@@ -9131,7 +9134,7 @@
         <v>2.6817567567567563E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A26" s="91" t="s">
         <v>78</v>
       </c>
@@ -9307,7 +9310,7 @@
         <v>2.1941646191646187E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A27" s="90" t="s">
         <v>6</v>
       </c>
@@ -9315,7 +9318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A28" s="91" t="s">
         <v>77</v>
       </c>
@@ -9491,7 +9494,7 @@
         <v>8.4922297297297292E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A29" s="91" t="s">
         <v>78</v>
       </c>
@@ -9667,7 +9670,7 @@
         <v>6.9481879606879599E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A30" s="90" t="s">
         <v>7</v>
       </c>
@@ -9717,7 +9720,7 @@
       <c r="AR30" s="92"/>
       <c r="AS30" s="92"/>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A31" s="91" t="s">
         <v>77</v>
       </c>
@@ -9893,7 +9896,7 @@
         <v>8.0878378378378378E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A32" s="91" t="s">
         <v>78</v>
       </c>
@@ -10069,7 +10072,7 @@
         <v>6.617321867321866E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A33" s="90" t="s">
         <v>12</v>
       </c>
@@ -10077,7 +10080,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A34" s="91" t="s">
         <v>77</v>
       </c>
@@ -10253,7 +10256,7 @@
         <v>7.5131756756756748E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A35" s="91" t="s">
         <v>78</v>
       </c>
@@ -10429,7 +10432,7 @@
         <v>6.1471437346437334E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="90" t="s">
         <v>81</v>
       </c>
@@ -10437,7 +10440,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A37" s="91" t="s">
         <v>77</v>
       </c>
@@ -10613,7 +10616,7 @@
         <v>0.31912905405405395</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A38" s="91" t="s">
         <v>78</v>
       </c>
@@ -10789,7 +10792,7 @@
         <v>0.26110558968058961</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A39" s="90" t="s">
         <v>92</v>
       </c>
@@ -10797,7 +10800,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A40" s="91" t="s">
         <v>77</v>
       </c>
@@ -10973,7 +10976,7 @@
         <v>0.12836249999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A41" s="91" t="s">
         <v>78</v>
       </c>
@@ -11149,7 +11152,7 @@
         <v>0.10502386363636362</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A42" s="90" t="s">
         <v>85</v>
       </c>
@@ -11199,7 +11202,7 @@
       <c r="AR42" s="92"/>
       <c r="AS42" s="92"/>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A43" s="91" t="s">
         <v>77</v>
       </c>
@@ -11376,7 +11379,7 @@
         <v>0.40896790540540534</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" s="91" t="s">
         <v>78</v>
       </c>
@@ -11552,7 +11555,7 @@
         <v>0.33461010442260436</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" s="89" t="s">
         <v>91</v>
       </c>
@@ -11560,7 +11563,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A47" s="90" t="s">
         <v>82</v>
       </c>
@@ -11694,7 +11697,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A48" s="91" t="s">
         <v>77</v>
       </c>
@@ -11849,7 +11852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A49" s="91" t="s">
         <v>78</v>
       </c>
@@ -12004,7 +12007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A50" s="90" t="s">
         <v>83</v>
       </c>
@@ -12033,7 +12036,7 @@
       <c r="AR50" s="92"/>
       <c r="AS50" s="92"/>
     </row>
-    <row r="51" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A51" s="91" t="s">
         <v>77</v>
       </c>
@@ -12188,7 +12191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A52" s="91" t="s">
         <v>78</v>
       </c>
@@ -12343,7 +12346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A53" s="90" t="s">
         <v>6</v>
       </c>
@@ -12372,7 +12375,7 @@
       <c r="AR53" s="92"/>
       <c r="AS53" s="92"/>
     </row>
-    <row r="54" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A54" s="91" t="s">
         <v>77</v>
       </c>
@@ -12527,7 +12530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A55" s="91" t="s">
         <v>78</v>
       </c>
@@ -12682,7 +12685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A56" s="90" t="s">
         <v>7</v>
       </c>
@@ -12732,7 +12735,7 @@
       <c r="AR56" s="92"/>
       <c r="AS56" s="92"/>
     </row>
-    <row r="57" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A57" s="91" t="s">
         <v>77</v>
       </c>
@@ -12887,7 +12890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A58" s="91" t="s">
         <v>78</v>
       </c>
@@ -13042,7 +13045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A59" s="90" t="s">
         <v>12</v>
       </c>
@@ -13050,7 +13053,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A60" s="91" t="s">
         <v>77</v>
       </c>
@@ -13226,7 +13229,7 @@
         <v>0.10641891891891891</v>
       </c>
     </row>
-    <row r="61" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A61" s="91" t="s">
         <v>78</v>
       </c>
@@ -13402,7 +13405,7 @@
         <v>8.7070024570024551E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A62" s="90" t="s">
         <v>81</v>
       </c>
@@ -13410,7 +13413,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A63" s="91" t="s">
         <v>77</v>
       </c>
@@ -13586,7 +13589,7 @@
         <v>0.31925675675675669</v>
       </c>
     </row>
-    <row r="64" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A64" s="91" t="s">
         <v>78</v>
       </c>
@@ -13762,7 +13765,7 @@
         <v>0.26121007371007371</v>
       </c>
     </row>
-    <row r="65" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A65" s="90" t="s">
         <v>92</v>
       </c>
@@ -13770,7 +13773,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="66" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A66" s="91" t="s">
         <v>77</v>
       </c>
@@ -13946,7 +13949,7 @@
         <v>0.21283783783783783</v>
       </c>
     </row>
-    <row r="67" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" s="91" t="s">
         <v>78</v>
       </c>
@@ -14122,7 +14125,7 @@
         <v>0.1741400491400491</v>
       </c>
     </row>
-    <row r="68" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" s="90" t="s">
         <v>85</v>
       </c>
@@ -14172,7 +14175,7 @@
       <c r="AR68" s="92"/>
       <c r="AS68" s="92"/>
     </row>
-    <row r="69" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" s="91" t="s">
         <v>77</v>
       </c>
@@ -14348,7 +14351,7 @@
         <v>0.42567567567567566</v>
       </c>
     </row>
-    <row r="70" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" s="91" t="s">
         <v>78</v>
       </c>
@@ -14524,12 +14527,12 @@
         <v>0.3482800982800982</v>
       </c>
     </row>
-    <row r="72" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" s="89" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" s="90" t="s">
         <v>82</v>
       </c>
@@ -14597,7 +14600,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" s="91" t="s">
         <v>77</v>
       </c>
@@ -14686,7 +14689,7 @@
         <v>1.4260135135135134E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A75" s="91" t="s">
         <v>78</v>
       </c>
@@ -14775,12 +14778,12 @@
         <v>1.1667383292383291E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A76" s="90" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A77" s="91" t="s">
         <v>77</v>
       </c>
@@ -14869,7 +14872,7 @@
         <v>4.3525337837837824E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A78" s="91" t="s">
         <v>78</v>
       </c>
@@ -14958,12 +14961,12 @@
         <v>3.5611640049140039E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A79" s="90" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A80" s="91" t="s">
         <v>77</v>
       </c>
@@ -15052,7 +15055,7 @@
         <v>8.2793918918918921E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" s="91" t="s">
         <v>78</v>
       </c>
@@ -15141,7 +15144,7 @@
         <v>6.7740479115479105E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" s="90" t="s">
         <v>7</v>
       </c>
@@ -15167,7 +15170,7 @@
       <c r="U82" s="92"/>
       <c r="V82" s="92"/>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" s="91" t="s">
         <v>77</v>
       </c>
@@ -15256,7 +15259,7 @@
         <v>7.8749999999999983E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" s="91" t="s">
         <v>78</v>
       </c>
@@ -15345,12 +15348,12 @@
         <v>6.4431818181818175E-3</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" s="90" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" s="91" t="s">
         <v>77</v>
       </c>
@@ -15439,7 +15442,7 @@
         <v>7.3216216216216212E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" s="91" t="s">
         <v>78</v>
       </c>
@@ -15528,12 +15531,12 @@
         <v>5.9904176904176897E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="90" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" s="91" t="s">
         <v>77</v>
       </c>
@@ -15622,7 +15625,7 @@
         <v>0.31107846283783785</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90" s="91" t="s">
         <v>78</v>
       </c>
@@ -15711,12 +15714,12 @@
         <v>0.25451874232186728</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A91" s="90" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A92" s="91" t="s">
         <v>77</v>
       </c>
@@ -15805,7 +15808,7 @@
         <v>0.1251326858108108</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93" s="91" t="s">
         <v>78</v>
       </c>
@@ -15894,7 +15897,7 @@
         <v>0.10238128839066338</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" s="90" t="s">
         <v>85</v>
       </c>
@@ -15920,7 +15923,7 @@
       <c r="U94" s="92"/>
       <c r="V94" s="92"/>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95" s="91" t="s">
         <v>77</v>
       </c>
@@ -16009,7 +16012,7 @@
         <v>0.39853885135135131</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" s="91" t="s">
         <v>78</v>
       </c>
@@ -16120,18 +16123,18 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>189</v>
       </c>
@@ -16157,7 +16160,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -16187,7 +16190,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -16217,7 +16220,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -16247,7 +16250,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="126" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" s="126" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="126" t="s">
         <v>7</v>
       </c>
@@ -16277,7 +16280,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -16307,7 +16310,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -16337,7 +16340,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -16367,7 +16370,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -16397,7 +16400,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F10" s="124">
         <v>0.8</v>
       </c>
@@ -16422,17 +16425,17 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="8" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="11" width="9.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="9.125" customWidth="1"/>
+    <col min="5" max="5" width="12.625" customWidth="1"/>
+    <col min="6" max="8" width="9.125" customWidth="1"/>
+    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="10" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="89" t="s">
         <v>125</v>
       </c>
@@ -16442,7 +16445,7 @@
       </c>
       <c r="E1" s="89"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="89" t="s">
         <v>123</v>
       </c>
@@ -16463,7 +16466,7 @@
       </c>
       <c r="H2" s="89"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -16482,7 +16485,7 @@
       </c>
       <c r="H3" s="119"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -16505,7 +16508,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -16534,7 +16537,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -16563,7 +16566,7 @@
         <v>7.98</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -16592,7 +16595,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -16621,7 +16624,7 @@
         <v>7.06</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -16650,7 +16653,7 @@
         <v>29.988</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -16680,7 +16683,7 @@
         <v>12.061999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -16711,7 +16714,7 @@
       </c>
       <c r="L11" s="142"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -16735,7 +16738,7 @@
       </c>
       <c r="L12" s="142"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -16758,7 +16761,7 @@
         <v>0.44983693240440503</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>135</v>
       </c>
@@ -16773,7 +16776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -16792,7 +16795,7 @@
         <v>0.81127894201174211</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -16815,7 +16818,7 @@
         <v>1.7090759647683011</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -16838,7 +16841,7 @@
         <v>0.76250611623046916</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -16861,7 +16864,7 @@
         <v>7.9823606349868017</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -16884,10 +16887,10 @@
         <v>0.75102385216179279</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H20" s="119"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>154</v>
       </c>
@@ -16919,17 +16922,17 @@
       <selection activeCell="J4" sqref="J4:J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="8" width="9.109375" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="11" width="9.109375" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="9.125" customWidth="1"/>
+    <col min="5" max="5" width="12.625" customWidth="1"/>
+    <col min="6" max="8" width="9.125" customWidth="1"/>
+    <col min="9" max="9" width="11.875" customWidth="1"/>
+    <col min="10" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" s="89" t="s">
         <v>125</v>
       </c>
@@ -16939,7 +16942,7 @@
       </c>
       <c r="E1" s="89"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="89" t="s">
         <v>123</v>
       </c>
@@ -16960,7 +16963,7 @@
       </c>
       <c r="H2" s="89"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -16979,7 +16982,7 @@
       </c>
       <c r="H3" s="119"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>127</v>
       </c>
@@ -17002,7 +17005,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -17031,7 +17034,7 @@
         <v>4.09</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -17060,7 +17063,7 @@
         <v>7.78</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -17089,7 +17092,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -17118,7 +17121,7 @@
         <v>6.88</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>131</v>
       </c>
@@ -17147,7 +17150,7 @@
         <v>29.2315</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -17177,7 +17180,7 @@
         <v>11.7585</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -17208,7 +17211,7 @@
       </c>
       <c r="L11" s="142"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -17232,7 +17235,7 @@
       </c>
       <c r="L12" s="142"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>134</v>
       </c>
@@ -17256,7 +17259,7 @@
         <v>1.3421630709048924</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>135</v>
       </c>
@@ -17271,7 +17274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>136</v>
       </c>
@@ -17290,7 +17293,7 @@
         <v>2.4205852337443363</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -17313,7 +17316,7 @@
         <v>1.6657750919960468</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -17336,7 +17339,7 @@
         <v>0.74318738434985454</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -17359,7 +17362,7 @@
         <v>7.7801208344144053</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -17382,10 +17385,10 @@
         <v>0.73199603307020844</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H20" s="119"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
         <v>154</v>
       </c>
@@ -17417,9 +17420,9 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="116" t="s">
         <v>108</v>
       </c>
@@ -17436,7 +17439,7 @@
         <v>59741.5010660794</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="116" t="s">
         <v>108</v>
       </c>
@@ -17453,7 +17456,7 @@
         <v>69138.670382745098</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="116" t="s">
         <v>108</v>
       </c>
@@ -17470,7 +17473,7 @@
         <v>80171.261562641506</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="116" t="s">
         <v>108</v>
       </c>
@@ -17487,7 +17490,7 @@
         <v>90432.492443495707</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="116" t="s">
         <v>108</v>
       </c>
@@ -17504,7 +17507,7 @@
         <v>99930.720481869299</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">
         <v>108</v>
       </c>
@@ -17521,7 +17524,7 @@
         <v>107983.575192006</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -17542,7 +17545,7 @@
         <v>9.5847204342851953</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -17563,7 +17566,7 @@
         <v>9.6858692480415378</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -17584,7 +17587,7 @@
         <v>9.7567805328937549</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -17605,7 +17608,7 @@
         <v>9.8164387304298284</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -17626,7 +17629,7 @@
         <v>9.9712261915638774</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>108</v>
       </c>
@@ -17647,7 +17650,7 @@
         <v>9.9451764906481976</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="116" t="s">
         <v>108</v>
       </c>
@@ -17664,7 +17667,7 @@
         <v>68984.546010035905</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="116" t="s">
         <v>108</v>
       </c>
@@ -17681,7 +17684,7 @@
         <v>82503.391937932494</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="116" t="s">
         <v>108</v>
       </c>
@@ -17698,7 +17701,7 @@
         <v>101358.072645382</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="116" t="s">
         <v>108</v>
       </c>
@@ -17715,7 +17718,7 @@
         <v>120942.68207155701</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="116" t="s">
         <v>108</v>
       </c>
@@ -17732,7 +17735,7 @@
         <v>141562.03003918901</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="116" t="s">
         <v>108</v>
       </c>
@@ -17749,7 +17752,7 @@
         <v>160171.573101469</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="116" t="s">
         <v>108</v>
       </c>
@@ -17770,7 +17773,7 @@
         <v>0.81157042900750931</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="116" t="s">
         <v>108</v>
       </c>
@@ -17791,7 +17794,7 @@
         <v>0.78909031045519518</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="116" t="s">
         <v>108</v>
       </c>
@@ -17812,7 +17815,7 @@
         <v>0.76163103415652622</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="116" t="s">
         <v>108</v>
       </c>
@@ -17833,7 +17836,7 @@
         <v>0.7412258471054296</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="116" t="s">
         <v>108</v>
       </c>
@@ -17854,7 +17857,7 @@
         <v>0.73045572993018792</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="116" t="s">
         <v>108</v>
       </c>
@@ -17875,7 +17878,7 @@
         <v>0.70826448737192038</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>114</v>
       </c>
@@ -17892,7 +17895,7 @@
         <v>5.7254886415853801E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -17909,7 +17912,7 @@
         <v>6.8778097933802795E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>114</v>
       </c>
@@ -17926,7 +17929,7 @@
         <v>7.9259287278305404E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -17943,7 +17946,7 @@
         <v>8.7911725763700405E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -17960,7 +17963,7 @@
         <v>9.6563852772143105E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -17977,7 +17980,7 @@
         <v>0.104223597161056</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -18002,7 +18005,7 @@
         <v>1.7646495534572713</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -18027,7 +18030,7 @@
         <v>1.8609945248532584</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -18052,7 +18055,7 @@
         <v>2.0341931821972952</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -18077,7 +18080,7 @@
         <v>2.1772007513285412</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>114</v>
       </c>
@@ -18102,7 +18105,7 @@
         <v>2.3089181346852699</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -18127,7 +18130,7 @@
         <v>2.3860580102167011</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -18144,7 +18147,7 @@
         <v>1043086.78450025</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>116</v>
       </c>
@@ -18161,7 +18164,7 @@
         <v>1004937.97850023</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -18178,7 +18181,7 @@
         <v>1011233.32315164</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>116</v>
       </c>
@@ -18195,7 +18198,7 @@
         <v>1028433.1229571101</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -18212,7 +18215,7 @@
         <v>1034649.3648125801</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>116</v>
       </c>
@@ -18229,7 +18232,7 @@
         <v>1035878.80248976</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -18250,7 +18253,7 @@
         <v>0.31108327811733788</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>116</v>
       </c>
@@ -18271,7 +18274,7 @@
         <v>0.35807604715171748</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>116</v>
       </c>
@@ -18292,7 +18295,7 @@
         <v>0.38026091329829254</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>116</v>
       </c>
@@ -18313,7 +18316,7 @@
         <v>0.3964641566230479</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>116</v>
       </c>
@@ -18334,7 +18337,7 @@
         <v>0.41710544227998719</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>116</v>
       </c>
@@ -18369,13 +18372,13 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="89" t="s">
         <v>181</v>
       </c>
@@ -18385,7 +18388,7 @@
       <c r="D1" s="89"/>
       <c r="E1" s="89"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -18402,7 +18405,7 @@
       <c r="G2" s="89"/>
       <c r="H2" s="89"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -18418,7 +18421,7 @@
       <c r="G3" s="142"/>
       <c r="H3" s="119"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -18435,7 +18438,7 @@
       <c r="H4" s="122"/>
       <c r="J4" s="48"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -18456,7 +18459,7 @@
       <c r="H5" s="122"/>
       <c r="J5" s="48"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -18474,7 +18477,7 @@
       <c r="H6" s="122"/>
       <c r="J6" s="48"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>137</v>
       </c>
@@ -18491,7 +18494,7 @@
       <c r="H7" s="122"/>
       <c r="J7" s="48"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>161</v>
       </c>
@@ -18508,7 +18511,7 @@
       <c r="H8" s="122"/>
       <c r="J8" s="48"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>162</v>
       </c>
@@ -18525,7 +18528,7 @@
       <c r="H9" s="122"/>
       <c r="J9" s="48"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>163</v>
       </c>
@@ -18546,7 +18549,7 @@
       <c r="H10" s="122"/>
       <c r="J10" s="48"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -18563,7 +18566,7 @@
       <c r="H11" s="122"/>
       <c r="J11" s="48"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>165</v>
       </c>
@@ -18579,7 +18582,7 @@
       </c>
       <c r="H12" s="122"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>166</v>
       </c>
@@ -18594,7 +18597,7 @@
       <c r="E13" s="144"/>
       <c r="H13" s="122"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>167</v>
       </c>
@@ -18609,7 +18612,7 @@
       <c r="E14" s="144"/>
       <c r="H14" s="122"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>168</v>
       </c>
@@ -18624,7 +18627,7 @@
       <c r="E15" s="144"/>
       <c r="H15" s="122"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>169</v>
       </c>
@@ -18638,7 +18641,7 @@
       <c r="E16" s="120"/>
       <c r="H16" s="122"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>170</v>
       </c>
@@ -18652,7 +18655,7 @@
       <c r="E17" s="120"/>
       <c r="H17" s="122"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -18666,7 +18669,7 @@
       <c r="E18" s="120"/>
       <c r="H18" s="122"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>172</v>
       </c>
@@ -18680,7 +18683,7 @@
       <c r="E19" s="120"/>
       <c r="H19" s="122"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>173</v>
       </c>
@@ -18693,7 +18696,7 @@
       </c>
       <c r="H20" s="119"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>174</v>
       </c>
@@ -18705,7 +18708,7 @@
         <v>2.5482093663911844</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>159</v>
       </c>
@@ -18717,7 +18720,7 @@
         <v>5.3374655647382916</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>175</v>
       </c>
@@ -18729,7 +18732,7 @@
         <v>2.3760330578512399</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -18741,7 +18744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -18753,7 +18756,7 @@
         <v>9.6763085399449036</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>176</v>
       </c>
@@ -18765,7 +18768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>177</v>
       </c>
@@ -18777,7 +18780,7 @@
         <v>4.0289256198347108</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>178</v>
       </c>
@@ -18789,7 +18792,7 @@
         <v>23.760330578512395</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>179</v>
       </c>
@@ -18797,7 +18800,7 @@
         <v>2904</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D31">
         <f>5/32</f>
         <v>0.15625</v>
@@ -18821,22 +18824,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>203</v>
       </c>
@@ -18859,7 +18862,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -18885,7 +18888,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -18911,7 +18914,7 @@
         <v>7.54</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -18937,7 +18940,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -18963,7 +18966,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -18989,7 +18992,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -19015,7 +19018,7 @@
         <v>46.11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -19041,7 +19044,7 @@
         <v>12.77</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>

</xml_diff>